<commit_message>
updated eye tracking study
</commit_message>
<xml_diff>
--- a/posts/bpd-young/bpd-young.xlsx
+++ b/posts/bpd-young/bpd-young.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/n_moopen_uu_nl/Documents/Documents/programming/doy-data-inventory/posts/bpd-young/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="11_AD4DB114E441178AC67DF4D4FE17F604683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AA0665F-C773-45C4-A6C2-D14257539C53}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="11_AD4DB114E441178AC67DF4D4FE17F604683EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{591E9364-3F48-4399-826E-1327EAF05B6D}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>CITATION METADATA</t>
   </si>
@@ -81,27 +81,18 @@
     <t>individuals</t>
   </si>
   <si>
-    <t>S-GGZ patients between 12-25 yeara of age; parents of the patients</t>
-  </si>
-  <si>
     <t>GGZ Centraal</t>
   </si>
   <si>
     <t>start of care + 2x follow-ups, 6 months apart</t>
   </si>
   <si>
-    <t>online questionnaire, filled out with the researcher standing by</t>
-  </si>
-  <si>
     <t>structured</t>
   </si>
   <si>
     <t>BPD YOUNG: DATA</t>
   </si>
   <si>
-    <t>A Person × Environment approach to Borderline Personality Disorder features in young people: The role of life events, parental support, and self-esteem</t>
-  </si>
-  <si>
     <t>The baseline dataset currently comprises 800 youth. The data is not openly available due to privacy considerations, the researchers can be contacted for further information and data access.</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>[Odilia Laucelle](o.m.laceulle@uu.nl) (Utrecht University)</t>
   </si>
   <si>
-    <t>Hessels, C.J., van den Berg, T., Lucassen, S.A. et al. Borderline personality disorder in young people: associations with support and negative interactions in relationships with mothers and a best friend. bord personal disord emot dysregul 9, 2 (2022). doi: &lt;https://doi.org/10.1186/s40479-021-00173-7&gt;</t>
-  </si>
-  <si>
     <t>_Start Date_: 2017-01-01</t>
   </si>
   <si>
@@ -193,6 +181,24 @@
   </si>
   <si>
     <t>**Data Collector**</t>
+  </si>
+  <si>
+    <t>S-GGZ patients between 12-25 years of age; parents of the patients</t>
+  </si>
+  <si>
+    <t>online questionnaire, filled out with the researcher on stand-by</t>
+  </si>
+  <si>
+    <t>Hessels, C.J., van den Berg, T., Lucassen, S.A. et al. Borderline personality disorder in young people: associations with support and negative interactions in relationships with mothers and a best friend. _bord personal disord emot dysregul_ *9*, 2 (2022). doi: &lt;https://doi.org/10.1186/s40479-021-00173-7&gt;</t>
+  </si>
+  <si>
+    <t>Hessels, C. J., de Moor, E. L., Deutz, M. H., Laceulle, O. M., &amp; Van Aken, M. A. (2024). Personality pathology in youth: A comparison of the categorical and alternative model in relation to internalizing and externalizing pathology and age-adequate psychosocial functioning. _Personality Disorders: Theory, Research, and Treatment, 15_(5), 293. doi: &lt;https://doi.org/10.1037/per0000681&gt;</t>
+  </si>
+  <si>
+    <t>de Groot, L. R., Hindriks, E., Hessels, C. J., van Aken, M. A., &amp; Laceulle, O. M. (2024). A Person× Environment approach to Borderline Personality Disorder features in young people: The role of life events, parental support, and self-esteem. _Journal of Social and Clinical Psychology, 43_(3), 276-301. doi: &lt;https://doi.org/10.1521/jscp.2024.43.3.276&gt;</t>
+  </si>
+  <si>
+    <t>Aleva, A., de Boois, G., Hessels, C. J., &amp; Laceulle, O. M. (2024). The Cross-Sectional and Longitudinal Associations between Household Chaos, Perceived Stress, and Borderline Personality Disorder Features in Outpatient Youth. _Youth, 4_(4), 1469-1480. &lt;https://doi.org/10.3390/youth4040093&gt;</t>
   </si>
 </sst>
 </file>
@@ -236,32 +242,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -546,273 +545,285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B24" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="B26" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B27" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="B28" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="B30" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="B32" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="B34" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="B35" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>